<commit_message>
organizando banco de dados
</commit_message>
<xml_diff>
--- a/respostas.xlsx
+++ b/respostas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\isabe\Documents\UFMG\6º período\Laboratório I\Parte2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7BB0A6F-97CF-48D7-AAF6-918C7592F659}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{536255DA-D2D0-4490-8141-3A2CDFBC7CF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6639" uniqueCount="1225">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6639" uniqueCount="1229">
   <si>
     <t>Carimbo de data/hora</t>
   </si>
@@ -3708,6 +3708,18 @@
   </si>
   <si>
     <t>Visita a patrimônios culturais exibidos na tela., Visita a parques, praças e espaços na natureza exibidos na tela., Desfrute da gastronomia retratada na tela, incluindo alimentos e bebidas., Visita a estabelecimentos exibidos na tela, como bares, restaurantes e outros., Outros</t>
+  </si>
+  <si>
+    <t>Outro</t>
+  </si>
+  <si>
+    <t>Outro, Encantamento</t>
+  </si>
+  <si>
+    <t>Autorrealização, Encantamento, Outro</t>
+  </si>
+  <si>
+    <t>Autorrealização, Nostalgia, Romance, Encantamento, Outro</t>
   </si>
 </sst>
 </file>
@@ -12877,14 +12889,14 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <sheetPr filterMode="1">
+  <sheetPr>
     <outlinePr summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:AE118"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="U1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="R119" sqref="R119"/>
+      <selection pane="bottomLeft" activeCell="Z1" sqref="Z1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5546875" defaultRowHeight="15.75" customHeight="1" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
@@ -12995,7 +13007,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:31" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A2" s="8">
         <v>44756.743593946754</v>
       </c>
@@ -13087,7 +13099,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="3" spans="1:31" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A3" s="8">
         <v>44756.746476273147</v>
       </c>
@@ -13179,7 +13191,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="4" spans="1:31" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A4" s="8">
         <v>44756.751307071754</v>
       </c>
@@ -13259,7 +13271,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="5" spans="1:31" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A5" s="8">
         <v>44756.751650844904</v>
       </c>
@@ -13351,7 +13363,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="6" spans="1:31" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A6" s="8">
         <v>44756.756480439813</v>
       </c>
@@ -13440,7 +13452,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="7" spans="1:31" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A7" s="8">
         <v>44756.765615289347</v>
       </c>
@@ -13535,7 +13547,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="8" spans="1:31" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A8" s="8">
         <v>44756.77190482639</v>
       </c>
@@ -13630,7 +13642,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="9" spans="1:31" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A9" s="8">
         <v>44756.781270081017</v>
       </c>
@@ -13722,7 +13734,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="10" spans="1:31" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A10" s="8">
         <v>44756.784393831018</v>
       </c>
@@ -13802,7 +13814,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="11" spans="1:31" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A11" s="8">
         <v>44756.788800416667</v>
       </c>
@@ -13882,7 +13894,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="12" spans="1:31" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A12" s="8">
         <v>44756.791462858797</v>
       </c>
@@ -13965,7 +13977,7 @@
         <v>954</v>
       </c>
     </row>
-    <row r="13" spans="1:31" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A13" s="8">
         <v>44756.795764756942</v>
       </c>
@@ -14054,7 +14066,7 @@
         <v>964</v>
       </c>
     </row>
-    <row r="14" spans="1:31" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A14" s="8">
         <v>44756.798618148146</v>
       </c>
@@ -14146,7 +14158,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="15" spans="1:31" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A15" s="8">
         <v>44756.799106678242</v>
       </c>
@@ -14229,7 +14241,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="16" spans="1:31" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A16" s="8">
         <v>44756.81055918982</v>
       </c>
@@ -14324,7 +14336,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="17" spans="1:31" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A17" s="8">
         <v>44756.816295104167</v>
       </c>
@@ -14416,7 +14428,7 @@
         <v>975</v>
       </c>
     </row>
-    <row r="18" spans="1:31" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A18" s="8">
         <v>44756.827279050922</v>
       </c>
@@ -14496,7 +14508,7 @@
         <v>982</v>
       </c>
     </row>
-    <row r="19" spans="1:31" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A19" s="8">
         <v>44756.836429988427</v>
       </c>
@@ -14579,7 +14591,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="20" spans="1:31" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A20" s="8">
         <v>44756.844614560185</v>
       </c>
@@ -14662,7 +14674,7 @@
         <v>989</v>
       </c>
     </row>
-    <row r="21" spans="1:31" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A21" s="8">
         <v>44756.871095520837</v>
       </c>
@@ -14748,7 +14760,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="22" spans="1:31" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A22" s="8">
         <v>44756.915538368055</v>
       </c>
@@ -14840,7 +14852,7 @@
         <v>999</v>
       </c>
     </row>
-    <row r="23" spans="1:31" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A23" s="8">
         <v>44756.915725775463</v>
       </c>
@@ -14935,7 +14947,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="24" spans="1:31" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A24" s="8">
         <v>44756.921014201391</v>
       </c>
@@ -15024,7 +15036,7 @@
         <v>1007</v>
       </c>
     </row>
-    <row r="25" spans="1:31" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A25" s="8">
         <v>44756.941017210644</v>
       </c>
@@ -15119,7 +15131,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="26" spans="1:31" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A26" s="8">
         <v>44756.942555740738</v>
       </c>
@@ -15211,7 +15223,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="27" spans="1:31" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A27" s="8">
         <v>44756.949555925923</v>
       </c>
@@ -15306,7 +15318,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="28" spans="1:31" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A28" s="8">
         <v>44756.97487351852</v>
       </c>
@@ -15398,7 +15410,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="29" spans="1:31" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A29" s="8">
         <v>44756.99139891204</v>
       </c>
@@ -15490,7 +15502,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="30" spans="1:31" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A30" s="8">
         <v>44756.996441898147</v>
       </c>
@@ -15585,7 +15597,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="31" spans="1:31" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A31" s="8">
         <v>44756.998882719912</v>
       </c>
@@ -15671,7 +15683,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="32" spans="1:31" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A32" s="8">
         <v>44757.336282847224</v>
       </c>
@@ -15757,7 +15769,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="33" spans="1:31" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A33" s="8">
         <v>44757.353061064816</v>
       </c>
@@ -15849,7 +15861,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="34" spans="1:31" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A34" s="8">
         <v>44757.367554224533</v>
       </c>
@@ -15932,7 +15944,7 @@
         <v>1024</v>
       </c>
     </row>
-    <row r="35" spans="1:31" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A35" s="8">
         <v>44757.37340394676</v>
       </c>
@@ -16021,7 +16033,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="36" spans="1:31" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A36" s="8">
         <v>44757.424635173607</v>
       </c>
@@ -16101,7 +16113,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="37" spans="1:31" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A37" s="8">
         <v>44757.425247453706</v>
       </c>
@@ -16196,7 +16208,7 @@
         <v>1034</v>
       </c>
     </row>
-    <row r="38" spans="1:31" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A38" s="8">
         <v>44757.485260335648</v>
       </c>
@@ -16249,7 +16261,7 @@
         <v>291</v>
       </c>
       <c r="T38" s="1" t="s">
-        <v>1039</v>
+        <v>1226</v>
       </c>
       <c r="U38" s="1" t="s">
         <v>74</v>
@@ -16285,7 +16297,7 @@
         <v>1044</v>
       </c>
     </row>
-    <row r="39" spans="1:31" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A39" s="8">
         <v>44757.514283750003</v>
       </c>
@@ -16368,7 +16380,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="40" spans="1:31" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A40" s="8">
         <v>44757.520848252316</v>
       </c>
@@ -16448,7 +16460,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="41" spans="1:31" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A41" s="8">
         <v>44757.537129490738</v>
       </c>
@@ -16540,7 +16552,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="42" spans="1:31" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A42" s="8">
         <v>44757.570692685185</v>
       </c>
@@ -16635,7 +16647,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="43" spans="1:31" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A43" s="8">
         <v>44757.577583460647</v>
       </c>
@@ -16727,7 +16739,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="44" spans="1:31" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A44" s="8">
         <v>44757.656166469911</v>
       </c>
@@ -16810,7 +16822,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="45" spans="1:31" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A45" s="8">
         <v>44757.775384513894</v>
       </c>
@@ -16890,7 +16902,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="46" spans="1:31" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A46" s="8">
         <v>44757.795752696758</v>
       </c>
@@ -16985,7 +16997,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="47" spans="1:31" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A47" s="8">
         <v>44757.842575543982</v>
       </c>
@@ -17041,7 +17053,7 @@
         <v>48</v>
       </c>
       <c r="T47" s="1" t="s">
-        <v>449</v>
+        <v>1225</v>
       </c>
       <c r="U47" s="1" t="s">
         <v>41</v>
@@ -17074,7 +17086,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="48" spans="1:31" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A48" s="8">
         <v>44758.725458171291</v>
       </c>
@@ -17157,7 +17169,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="49" spans="1:31" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A49" s="8">
         <v>44759.705415173608</v>
       </c>
@@ -17243,7 +17255,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="50" spans="1:31" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A50" s="8">
         <v>44760.010943865738</v>
       </c>
@@ -17335,7 +17347,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="51" spans="1:31" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A51" s="8">
         <v>44760.399100844908</v>
       </c>
@@ -17421,7 +17433,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="52" spans="1:31" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A52" s="8">
         <v>44760.408561296295</v>
       </c>
@@ -17513,7 +17525,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="53" spans="1:31" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A53" s="8">
         <v>44760.506068842587</v>
       </c>
@@ -17608,7 +17620,7 @@
         <v>503</v>
       </c>
     </row>
-    <row r="54" spans="1:31" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A54" s="8">
         <v>44760.55148765046</v>
       </c>
@@ -17697,7 +17709,7 @@
         <v>1062</v>
       </c>
     </row>
-    <row r="55" spans="1:31" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A55" s="8">
         <v>44760.560046250001</v>
       </c>
@@ -17792,7 +17804,7 @@
         <v>516</v>
       </c>
     </row>
-    <row r="56" spans="1:31" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A56" s="8">
         <v>44760.628381087961</v>
       </c>
@@ -17887,7 +17899,7 @@
         <v>1073</v>
       </c>
     </row>
-    <row r="57" spans="1:31" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A57" s="8">
         <v>44760.652184699073</v>
       </c>
@@ -17982,7 +17994,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="58" spans="1:31" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A58" s="8">
         <v>44760.65833395833</v>
       </c>
@@ -18065,7 +18077,7 @@
         <v>1081</v>
       </c>
     </row>
-    <row r="59" spans="1:31" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A59" s="8">
         <v>44760.738571678245</v>
       </c>
@@ -18157,7 +18169,7 @@
         <v>539</v>
       </c>
     </row>
-    <row r="60" spans="1:31" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A60" s="8">
         <v>44760.80759113426</v>
       </c>
@@ -18240,7 +18252,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="61" spans="1:31" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A61" s="8">
         <v>44761.400200868055</v>
       </c>
@@ -18335,7 +18347,7 @@
         <v>1091</v>
       </c>
     </row>
-    <row r="62" spans="1:31" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A62" s="8">
         <v>44761.730599513889</v>
       </c>
@@ -18430,7 +18442,7 @@
         <v>559</v>
       </c>
     </row>
-    <row r="63" spans="1:31" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A63" s="8">
         <v>44762.615112916668</v>
       </c>
@@ -18504,7 +18516,7 @@
         <v>563</v>
       </c>
     </row>
-    <row r="64" spans="1:31" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A64" s="8">
         <v>44762.778823912042</v>
       </c>
@@ -18596,7 +18608,7 @@
         <v>1102</v>
       </c>
     </row>
-    <row r="65" spans="1:31" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A65" s="8">
         <v>44763.178732187502</v>
       </c>
@@ -18688,7 +18700,7 @@
         <v>574</v>
       </c>
     </row>
-    <row r="66" spans="1:31" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A66" s="8">
         <v>44763.281734722223</v>
       </c>
@@ -18765,7 +18777,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="67" spans="1:31" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A67" s="8">
         <v>44763.328978657402</v>
       </c>
@@ -18845,7 +18857,7 @@
         <v>588</v>
       </c>
     </row>
-    <row r="68" spans="1:31" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A68" s="8">
         <v>44763.354922604165</v>
       </c>
@@ -18925,7 +18937,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="69" spans="1:31" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A69" s="8">
         <v>44763.411183414355</v>
       </c>
@@ -19014,7 +19026,7 @@
         <v>605</v>
       </c>
     </row>
-    <row r="70" spans="1:31" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A70" s="8">
         <v>44763.429527500004</v>
       </c>
@@ -19094,7 +19106,7 @@
         <v>611</v>
       </c>
     </row>
-    <row r="71" spans="1:31" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A71" s="8">
         <v>44763.436787152779</v>
       </c>
@@ -19189,7 +19201,7 @@
         <v>622</v>
       </c>
     </row>
-    <row r="72" spans="1:31" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A72" s="8">
         <v>44763.598419664355</v>
       </c>
@@ -19272,7 +19284,7 @@
         <v>629</v>
       </c>
     </row>
-    <row r="73" spans="1:31" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A73" s="8">
         <v>44763.637512650464</v>
       </c>
@@ -19355,7 +19367,7 @@
         <v>644</v>
       </c>
     </row>
-    <row r="74" spans="1:31" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A74" s="8">
         <v>44763.6417515625</v>
       </c>
@@ -19450,7 +19462,7 @@
         <v>657</v>
       </c>
     </row>
-    <row r="75" spans="1:31" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A75" s="8">
         <v>44763.663818275461</v>
       </c>
@@ -19530,7 +19542,7 @@
         <v>1109</v>
       </c>
     </row>
-    <row r="76" spans="1:31" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A76" s="8">
         <v>44763.671027303237</v>
       </c>
@@ -19619,7 +19631,7 @@
         <v>667</v>
       </c>
     </row>
-    <row r="77" spans="1:31" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A77" s="8">
         <v>44763.681260590281</v>
       </c>
@@ -19708,7 +19720,7 @@
         <v>675</v>
       </c>
     </row>
-    <row r="78" spans="1:31" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A78" s="8">
         <v>44763.683786527778</v>
       </c>
@@ -19782,7 +19794,7 @@
         <v>680</v>
       </c>
     </row>
-    <row r="79" spans="1:31" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A79" s="8">
         <v>44763.710078159726</v>
       </c>
@@ -19877,7 +19889,7 @@
         <v>693</v>
       </c>
     </row>
-    <row r="80" spans="1:31" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A80" s="8">
         <v>44763.751637106485</v>
       </c>
@@ -19966,7 +19978,7 @@
         <v>705</v>
       </c>
     </row>
-    <row r="81" spans="1:31" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A81" s="8">
         <v>44763.75527415509</v>
       </c>
@@ -20058,7 +20070,7 @@
         <v>1119</v>
       </c>
     </row>
-    <row r="82" spans="1:31" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A82" s="8">
         <v>44763.821287812505</v>
       </c>
@@ -20135,7 +20147,7 @@
         <v>711</v>
       </c>
     </row>
-    <row r="83" spans="1:31" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A83" s="8">
         <v>44763.837111412038</v>
       </c>
@@ -20230,7 +20242,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="84" spans="1:31" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A84" s="8">
         <v>44764.037820069439</v>
       </c>
@@ -20325,7 +20337,7 @@
         <v>728</v>
       </c>
     </row>
-    <row r="85" spans="1:31" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A85" s="8">
         <v>44764.375806331023</v>
       </c>
@@ -20411,7 +20423,7 @@
         <v>736</v>
       </c>
     </row>
-    <row r="86" spans="1:31" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A86" s="8">
         <v>44764.440489525463</v>
       </c>
@@ -20497,7 +20509,7 @@
         <v>1126</v>
       </c>
     </row>
-    <row r="87" spans="1:31" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A87" s="8">
         <v>44765.376572546294</v>
       </c>
@@ -20586,7 +20598,7 @@
         <v>741</v>
       </c>
     </row>
-    <row r="88" spans="1:31" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A88" s="8">
         <v>44767.342136134263</v>
       </c>
@@ -20678,7 +20690,7 @@
         <v>749</v>
       </c>
     </row>
-    <row r="89" spans="1:31" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A89" s="8">
         <v>44767.408527858795</v>
       </c>
@@ -20758,7 +20770,7 @@
         <v>758</v>
       </c>
     </row>
-    <row r="90" spans="1:31" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A90" s="8">
         <v>44767.786165798607</v>
       </c>
@@ -20847,7 +20859,7 @@
         <v>768</v>
       </c>
     </row>
-    <row r="91" spans="1:31" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A91" s="8">
         <v>44767.982161064814</v>
       </c>
@@ -20942,7 +20954,7 @@
         <v>778</v>
       </c>
     </row>
-    <row r="92" spans="1:31" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A92" s="8">
         <v>44768.49386505787</v>
       </c>
@@ -21028,7 +21040,7 @@
         <v>785</v>
       </c>
     </row>
-    <row r="93" spans="1:31" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A93" s="8">
         <v>44768.961886979167</v>
       </c>
@@ -21108,7 +21120,7 @@
         <v>1134</v>
       </c>
     </row>
-    <row r="94" spans="1:31" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A94" s="8">
         <v>44769.551213599538</v>
       </c>
@@ -21188,7 +21200,7 @@
         <v>1139</v>
       </c>
     </row>
-    <row r="95" spans="1:31" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A95" s="8">
         <v>44769.591317662038</v>
       </c>
@@ -21268,7 +21280,7 @@
         <v>792</v>
       </c>
     </row>
-    <row r="96" spans="1:31" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A96" s="8">
         <v>44769.614276805558</v>
       </c>
@@ -21354,7 +21366,7 @@
         <v>799</v>
       </c>
     </row>
-    <row r="97" spans="1:31" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A97" s="8">
         <v>44769.618707048612</v>
       </c>
@@ -21437,7 +21449,7 @@
         <v>807</v>
       </c>
     </row>
-    <row r="98" spans="1:31" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A98" s="8">
         <v>44772.587381527774</v>
       </c>
@@ -21526,7 +21538,7 @@
         <v>1150</v>
       </c>
     </row>
-    <row r="99" spans="1:31" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A99" s="8">
         <v>44773.372072673606</v>
       </c>
@@ -21618,7 +21630,7 @@
         <v>816</v>
       </c>
     </row>
-    <row r="100" spans="1:31" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A100" s="8">
         <v>44774.051016979167</v>
       </c>
@@ -21713,7 +21725,7 @@
         <v>827</v>
       </c>
     </row>
-    <row r="101" spans="1:31" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A101" s="8">
         <v>44774.702917187504</v>
       </c>
@@ -21805,7 +21817,7 @@
         <v>836</v>
       </c>
     </row>
-    <row r="102" spans="1:31" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A102" s="8">
         <v>44774.732120659726</v>
       </c>
@@ -21891,7 +21903,7 @@
         <v>844</v>
       </c>
     </row>
-    <row r="103" spans="1:31" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A103" s="8">
         <v>44774.834338275468</v>
       </c>
@@ -21968,7 +21980,7 @@
         <v>852</v>
       </c>
     </row>
-    <row r="104" spans="1:31" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A104" s="8">
         <v>44774.980285393518</v>
       </c>
@@ -22045,7 +22057,7 @@
         <v>858</v>
       </c>
     </row>
-    <row r="105" spans="1:31" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A105" s="8">
         <v>44775.595694606483</v>
       </c>
@@ -22140,7 +22152,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="106" spans="1:31" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A106" s="8">
         <v>44783.63758840278</v>
       </c>
@@ -22235,7 +22247,7 @@
         <v>879</v>
       </c>
     </row>
-    <row r="107" spans="1:31" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A107" s="8">
         <v>44783.682308530093</v>
       </c>
@@ -22386,7 +22398,7 @@
         <v>888</v>
       </c>
       <c r="T108" s="1" t="s">
-        <v>889</v>
+        <v>1227</v>
       </c>
       <c r="U108" s="1" t="s">
         <v>41</v>
@@ -22422,7 +22434,7 @@
         <v>894</v>
       </c>
     </row>
-    <row r="109" spans="1:31" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A109" s="8">
         <v>44784.349818946765</v>
       </c>
@@ -22514,7 +22526,7 @@
         <v>1169</v>
       </c>
     </row>
-    <row r="110" spans="1:31" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A110" s="8">
         <v>44784.535158125</v>
       </c>
@@ -22573,7 +22585,7 @@
         <v>291</v>
       </c>
       <c r="T110" s="1" t="s">
-        <v>898</v>
+        <v>1228</v>
       </c>
       <c r="U110" s="1" t="s">
         <v>41</v>
@@ -22606,7 +22618,7 @@
         <v>902</v>
       </c>
     </row>
-    <row r="111" spans="1:31" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A111" s="8">
         <v>44784.55242501157</v>
       </c>
@@ -22701,7 +22713,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="112" spans="1:31" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A112" s="8">
         <v>44785.054983888884</v>
       </c>
@@ -22787,7 +22799,7 @@
         <v>919</v>
       </c>
     </row>
-    <row r="113" spans="1:31" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A113" s="8">
         <v>44785.523622499997</v>
       </c>
@@ -22867,7 +22879,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="114" spans="1:31" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A114" s="8">
         <v>44789.386663738427</v>
       </c>
@@ -22959,7 +22971,7 @@
         <v>1183</v>
       </c>
     </row>
-    <row r="115" spans="1:31" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A115" s="8">
         <v>44795.453067465278</v>
       </c>
@@ -23042,7 +23054,7 @@
         <v>926</v>
       </c>
     </row>
-    <row r="116" spans="1:31" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A116" s="8">
         <v>44797.964524814815</v>
       </c>
@@ -23134,7 +23146,7 @@
         <v>936</v>
       </c>
     </row>
-    <row r="117" spans="1:31" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A117" s="8">
         <v>44798.701526782403</v>
       </c>
@@ -23223,7 +23235,7 @@
         <v>1191</v>
       </c>
     </row>
-    <row r="118" spans="1:31" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A118" s="8">
         <v>44799.579709247686</v>
       </c>
@@ -23313,23 +23325,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" ref="A1:AK118" xr:uid="{00000000-0009-0000-0000-000002000000}">
-    <filterColumn colId="17">
-      <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-        <mc:Choice Requires="x14">
-          <filters>
-            <x14:filter val="Visita a patrimônios culturais exibidos na tela., Visita a parques, praças e espaços na natureza exibidos na tela., Desfrute da gastronomia retratada na tela, incluindo alimentos e bebidas., Visita a estabelecimentos exibidos na tela, como bares, restaurantes e outros., Praias"/>
-          </filters>
-        </mc:Choice>
-        <mc:Fallback>
-          <customFilters>
-            <customFilter val=""/>
-            <customFilter operator="notEqual" val=" "/>
-          </customFilters>
-        </mc:Fallback>
-      </mc:AlternateContent>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:AK118" xr:uid="{00000000-0009-0000-0000-000002000000}"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Organização do banco, elaboração dos gráficos e teste qui-quadrado logo abaixo dos gráficos.
Falta terminar as análises para result2
</commit_message>
<xml_diff>
--- a/respostas.xlsx
+++ b/respostas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\isabe\Documents\UFMG\6º período\Laboratório I\Parte2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{536255DA-D2D0-4490-8141-3A2CDFBC7CF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3027825-650C-42D7-8524-5D1924587653}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6639" uniqueCount="1229">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6639" uniqueCount="1228">
   <si>
     <t>Carimbo de data/hora</t>
   </si>
@@ -3702,9 +3702,6 @@
   </si>
   <si>
     <t>Netflix, Amazon Prime Vídeo, Outros</t>
-  </si>
-  <si>
-    <t>Outros (Audiovisual)</t>
   </si>
   <si>
     <t>Visita a patrimônios culturais exibidos na tela., Visita a parques, praças e espaços na natureza exibidos na tela., Desfrute da gastronomia retratada na tela, incluindo alimentos e bebidas., Visita a estabelecimentos exibidos na tela, como bares, restaurantes e outros., Outros</t>
@@ -3729,7 +3726,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m/d/yyyy\ h:mm:ss"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -3740,6 +3737,13 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -3781,7 +3785,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
@@ -3791,6 +3795,7 @@
     <xf numFmtId="164" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -12894,17 +12899,17 @@
   </sheetPr>
   <dimension ref="A1:AE118"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="U1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="V1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Z1" sqref="Z1"/>
+      <selection pane="bottomLeft" activeCell="Z6" sqref="Z6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5546875" defaultRowHeight="15.75" customHeight="1" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="12" width="18.88671875" customWidth="1"/>
-    <col min="13" max="13" width="39.33203125" customWidth="1"/>
-    <col min="14" max="14" width="136.44140625" customWidth="1"/>
-    <col min="15" max="15" width="88.109375" customWidth="1"/>
+    <col min="13" max="13" width="39.33203125" hidden="1" customWidth="1"/>
+    <col min="14" max="14" width="16.33203125" customWidth="1"/>
+    <col min="15" max="15" width="88.109375" hidden="1" customWidth="1"/>
     <col min="16" max="23" width="18.88671875" customWidth="1"/>
     <col min="24" max="24" width="17" customWidth="1"/>
     <col min="25" max="25" width="63.88671875" customWidth="1"/>
@@ -14023,8 +14028,8 @@
       <c r="O13" s="1" t="s">
         <v>959</v>
       </c>
-      <c r="P13" s="1" t="s">
-        <v>1223</v>
+      <c r="P13" s="9" t="s">
+        <v>46</v>
       </c>
       <c r="Q13" s="1" t="s">
         <v>678</v>
@@ -16261,7 +16266,7 @@
         <v>291</v>
       </c>
       <c r="T38" s="1" t="s">
-        <v>1226</v>
+        <v>1225</v>
       </c>
       <c r="U38" s="1" t="s">
         <v>74</v>
@@ -17053,7 +17058,7 @@
         <v>48</v>
       </c>
       <c r="T47" s="1" t="s">
-        <v>1225</v>
+        <v>1224</v>
       </c>
       <c r="U47" s="1" t="s">
         <v>41</v>
@@ -17666,8 +17671,8 @@
       <c r="O54" s="1" t="s">
         <v>1055</v>
       </c>
-      <c r="P54" s="1" t="s">
-        <v>1223</v>
+      <c r="P54" s="9" t="s">
+        <v>46</v>
       </c>
       <c r="Q54" s="1" t="s">
         <v>1057</v>
@@ -18298,8 +18303,8 @@
       <c r="O61" s="1" t="s">
         <v>1084</v>
       </c>
-      <c r="P61" s="1" t="s">
-        <v>1223</v>
+      <c r="P61" s="9" t="s">
+        <v>46</v>
       </c>
       <c r="Q61" s="1" t="s">
         <v>1086</v>
@@ -21495,8 +21500,8 @@
       <c r="O98" s="1" t="s">
         <v>1144</v>
       </c>
-      <c r="P98" s="1" t="s">
-        <v>1223</v>
+      <c r="P98" s="9" t="s">
+        <v>46</v>
       </c>
       <c r="Q98" s="1" t="s">
         <v>678</v>
@@ -22392,13 +22397,13 @@
         <v>886</v>
       </c>
       <c r="R108" s="1" t="s">
-        <v>1224</v>
+        <v>1223</v>
       </c>
       <c r="S108" s="1" t="s">
         <v>888</v>
       </c>
       <c r="T108" s="1" t="s">
-        <v>1227</v>
+        <v>1226</v>
       </c>
       <c r="U108" s="1" t="s">
         <v>41</v>
@@ -22585,7 +22590,7 @@
         <v>291</v>
       </c>
       <c r="T110" s="1" t="s">
-        <v>1228</v>
+        <v>1227</v>
       </c>
       <c r="U110" s="1" t="s">
         <v>41</v>

</xml_diff>

<commit_message>
- Organização do banco completa; - Feito testes qui-quadrado para cada variável e gráfico; - Única variável significativa: filmes
</commit_message>
<xml_diff>
--- a/respostas.xlsx
+++ b/respostas.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\isabe\Documents\UFMG\6º período\Laboratório I\Parte2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\m755263\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3027825-650C-42D7-8524-5D1924587653}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="10500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Respostas ao formulário 2" sheetId="1" r:id="rId1"/>
@@ -28,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6639" uniqueCount="1228">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6639" uniqueCount="1227">
   <si>
     <t>Carimbo de data/hora</t>
   </si>
@@ -3707,22 +3706,19 @@
     <t>Visita a patrimônios culturais exibidos na tela., Visita a parques, praças e espaços na natureza exibidos na tela., Desfrute da gastronomia retratada na tela, incluindo alimentos e bebidas., Visita a estabelecimentos exibidos na tela, como bares, restaurantes e outros., Outros</t>
   </si>
   <si>
-    <t>Outro</t>
-  </si>
-  <si>
-    <t>Outro, Encantamento</t>
-  </si>
-  <si>
-    <t>Autorrealização, Encantamento, Outro</t>
-  </si>
-  <si>
-    <t>Autorrealização, Nostalgia, Romance, Encantamento, Outro</t>
+    <t>Outros, Encantamento</t>
+  </si>
+  <si>
+    <t>Autorrealização, Encantamento, Outros</t>
+  </si>
+  <si>
+    <t>Autorrealização, Nostalgia, Romance, Encantamento, Outros</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m/d/yyyy\ h:mm:ss"/>
   </numFmts>
@@ -4010,7 +4006,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
@@ -4021,12 +4017,12 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5546875" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="8" width="18.88671875" customWidth="1"/>
+    <col min="1" max="8" width="18.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4040,7 +4036,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF0000FF"/>
     <outlinePr summaryRight="0"/>
@@ -4052,19 +4048,19 @@
       <selection pane="bottomLeft" activeCell="P92" sqref="P92"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5546875" defaultRowHeight="15.75" customHeight="1" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" outlineLevelRow="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="13" width="18.88671875" customWidth="1"/>
-    <col min="14" max="14" width="136.44140625" customWidth="1"/>
-    <col min="15" max="15" width="88.109375" customWidth="1"/>
-    <col min="16" max="16" width="69.44140625" customWidth="1"/>
-    <col min="17" max="17" width="123.5546875" customWidth="1"/>
-    <col min="18" max="18" width="18.88671875" customWidth="1"/>
-    <col min="19" max="19" width="122.6640625" customWidth="1"/>
-    <col min="20" max="37" width="18.88671875" customWidth="1"/>
+    <col min="1" max="13" width="18.85546875" customWidth="1"/>
+    <col min="14" max="14" width="136.42578125" customWidth="1"/>
+    <col min="15" max="15" width="88.140625" customWidth="1"/>
+    <col min="16" max="16" width="69.42578125" customWidth="1"/>
+    <col min="17" max="17" width="123.5703125" customWidth="1"/>
+    <col min="18" max="18" width="18.85546875" customWidth="1"/>
+    <col min="19" max="19" width="122.7109375" customWidth="1"/>
+    <col min="20" max="37" width="18.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37" ht="13.2" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:37" ht="12.75" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4159,7 +4155,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:37" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>44756.743593946754</v>
       </c>
@@ -4258,7 +4254,7 @@
       <c r="AJ2" s="3"/>
       <c r="AK2" s="3"/>
     </row>
-    <row r="3" spans="1:37" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A3" s="4">
         <v>44756.746476273147</v>
       </c>
@@ -4357,7 +4353,7 @@
       <c r="AJ3" s="5"/>
       <c r="AK3" s="5"/>
     </row>
-    <row r="4" spans="1:37" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A4" s="4">
         <v>44756.751307071754</v>
       </c>
@@ -4448,7 +4444,7 @@
       <c r="AJ4" s="5"/>
       <c r="AK4" s="5"/>
     </row>
-    <row r="5" spans="1:37" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A5" s="4">
         <v>44756.751650844904</v>
       </c>
@@ -4547,7 +4543,7 @@
       <c r="AJ5" s="5"/>
       <c r="AK5" s="5"/>
     </row>
-    <row r="6" spans="1:37" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>44756.756480439813</v>
       </c>
@@ -4644,7 +4640,7 @@
       <c r="AJ6" s="3"/>
       <c r="AK6" s="3"/>
     </row>
-    <row r="7" spans="1:37" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>44756.765615289347</v>
       </c>
@@ -4745,7 +4741,7 @@
       <c r="AJ7" s="3"/>
       <c r="AK7" s="3"/>
     </row>
-    <row r="8" spans="1:37" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>44756.77190482639</v>
       </c>
@@ -4846,7 +4842,7 @@
       <c r="AJ8" s="3"/>
       <c r="AK8" s="3"/>
     </row>
-    <row r="9" spans="1:37" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>44756.781270081017</v>
       </c>
@@ -4945,7 +4941,7 @@
       <c r="AJ9" s="3"/>
       <c r="AK9" s="3"/>
     </row>
-    <row r="10" spans="1:37" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A10" s="4">
         <v>44756.784393831018</v>
       </c>
@@ -5036,7 +5032,7 @@
       <c r="AJ10" s="5"/>
       <c r="AK10" s="5"/>
     </row>
-    <row r="11" spans="1:37" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <v>44756.788800416667</v>
       </c>
@@ -5127,7 +5123,7 @@
       <c r="AJ11" s="3"/>
       <c r="AK11" s="3"/>
     </row>
-    <row r="12" spans="1:37" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A12" s="4">
         <v>44756.798618148146</v>
       </c>
@@ -5226,7 +5222,7 @@
       <c r="AJ12" s="5"/>
       <c r="AK12" s="5"/>
     </row>
-    <row r="13" spans="1:37" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A13" s="4">
         <v>44756.799106678242</v>
       </c>
@@ -5319,7 +5315,7 @@
       <c r="AJ13" s="5"/>
       <c r="AK13" s="5"/>
     </row>
-    <row r="14" spans="1:37" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A14" s="4">
         <v>44756.81055918982</v>
       </c>
@@ -5420,7 +5416,7 @@
       <c r="AJ14" s="5"/>
       <c r="AK14" s="5"/>
     </row>
-    <row r="15" spans="1:37" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A15" s="4">
         <v>44756.836429988427</v>
       </c>
@@ -5513,7 +5509,7 @@
       <c r="AJ15" s="5"/>
       <c r="AK15" s="5"/>
     </row>
-    <row r="16" spans="1:37" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
         <v>44756.871095520837</v>
       </c>
@@ -5608,7 +5604,7 @@
       <c r="AJ16" s="3"/>
       <c r="AK16" s="3"/>
     </row>
-    <row r="17" spans="1:37" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A17" s="4">
         <v>44756.915725775463</v>
       </c>
@@ -5709,7 +5705,7 @@
       <c r="AJ17" s="5"/>
       <c r="AK17" s="5"/>
     </row>
-    <row r="18" spans="1:37" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
         <v>44756.941017210644</v>
       </c>
@@ -5810,7 +5806,7 @@
       <c r="AJ18" s="3"/>
       <c r="AK18" s="3"/>
     </row>
-    <row r="19" spans="1:37" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:37" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="4">
         <v>44756.942555740738</v>
       </c>
@@ -5909,7 +5905,7 @@
       <c r="AJ19" s="5"/>
       <c r="AK19" s="5"/>
     </row>
-    <row r="20" spans="1:37" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A20" s="2">
         <v>44756.949555925923</v>
       </c>
@@ -6010,7 +6006,7 @@
       <c r="AJ20" s="3"/>
       <c r="AK20" s="3"/>
     </row>
-    <row r="21" spans="1:37" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A21" s="4">
         <v>44756.99139891204</v>
       </c>
@@ -6109,7 +6105,7 @@
       <c r="AJ21" s="5"/>
       <c r="AK21" s="5"/>
     </row>
-    <row r="22" spans="1:37" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A22" s="4">
         <v>44756.996441898147</v>
       </c>
@@ -6210,7 +6206,7 @@
       <c r="AJ22" s="5"/>
       <c r="AK22" s="5"/>
     </row>
-    <row r="23" spans="1:37" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A23" s="4">
         <v>44756.998882719912</v>
       </c>
@@ -6305,7 +6301,7 @@
       <c r="AJ23" s="5"/>
       <c r="AK23" s="5"/>
     </row>
-    <row r="24" spans="1:37" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A24" s="4">
         <v>44757.336282847224</v>
       </c>
@@ -6400,7 +6396,7 @@
       <c r="AJ24" s="5"/>
       <c r="AK24" s="5"/>
     </row>
-    <row r="25" spans="1:37" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A25" s="4">
         <v>44757.353061064816</v>
       </c>
@@ -6499,7 +6495,7 @@
       <c r="AJ25" s="5"/>
       <c r="AK25" s="5"/>
     </row>
-    <row r="26" spans="1:37" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A26" s="2">
         <v>44757.37340394676</v>
       </c>
@@ -6596,7 +6592,7 @@
       <c r="AJ26" s="3"/>
       <c r="AK26" s="3"/>
     </row>
-    <row r="27" spans="1:37" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A27" s="4">
         <v>44757.424635173607</v>
       </c>
@@ -6687,7 +6683,7 @@
       <c r="AJ27" s="5"/>
       <c r="AK27" s="5"/>
     </row>
-    <row r="28" spans="1:37" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A28" s="4">
         <v>44757.514283750003</v>
       </c>
@@ -6780,7 +6776,7 @@
       <c r="AJ28" s="5"/>
       <c r="AK28" s="5"/>
     </row>
-    <row r="29" spans="1:37" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A29" s="4">
         <v>44757.520848252316</v>
       </c>
@@ -6871,7 +6867,7 @@
       <c r="AJ29" s="5"/>
       <c r="AK29" s="5"/>
     </row>
-    <row r="30" spans="1:37" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A30" s="4">
         <v>44757.537129490738</v>
       </c>
@@ -6970,7 +6966,7 @@
       <c r="AJ30" s="5"/>
       <c r="AK30" s="5"/>
     </row>
-    <row r="31" spans="1:37" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A31" s="4">
         <v>44757.570692685185</v>
       </c>
@@ -7071,7 +7067,7 @@
       <c r="AJ31" s="5"/>
       <c r="AK31" s="5"/>
     </row>
-    <row r="32" spans="1:37" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A32" s="2">
         <v>44757.577583460647</v>
       </c>
@@ -7170,7 +7166,7 @@
       <c r="AJ32" s="3"/>
       <c r="AK32" s="3"/>
     </row>
-    <row r="33" spans="1:37" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A33" s="2">
         <v>44757.656166469911</v>
       </c>
@@ -7263,7 +7259,7 @@
       <c r="AJ33" s="3"/>
       <c r="AK33" s="3"/>
     </row>
-    <row r="34" spans="1:37" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A34" s="4">
         <v>44757.775384513894</v>
       </c>
@@ -7354,7 +7350,7 @@
       <c r="AJ34" s="5"/>
       <c r="AK34" s="5"/>
     </row>
-    <row r="35" spans="1:37" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A35" s="4">
         <v>44757.795752696758</v>
       </c>
@@ -7455,7 +7451,7 @@
       <c r="AJ35" s="5"/>
       <c r="AK35" s="5"/>
     </row>
-    <row r="36" spans="1:37" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A36" s="2">
         <v>44757.842575543982</v>
       </c>
@@ -7552,7 +7548,7 @@
       <c r="AJ36" s="3"/>
       <c r="AK36" s="3"/>
     </row>
-    <row r="37" spans="1:37" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A37" s="4">
         <v>44758.725458171291</v>
       </c>
@@ -7645,7 +7641,7 @@
       <c r="AJ37" s="5"/>
       <c r="AK37" s="5"/>
     </row>
-    <row r="38" spans="1:37" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A38" s="4">
         <v>44760.010943865738</v>
       </c>
@@ -7744,7 +7740,7 @@
       <c r="AJ38" s="5"/>
       <c r="AK38" s="5"/>
     </row>
-    <row r="39" spans="1:37" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A39" s="2">
         <v>44760.399100844908</v>
       </c>
@@ -7839,7 +7835,7 @@
       <c r="AJ39" s="3"/>
       <c r="AK39" s="3"/>
     </row>
-    <row r="40" spans="1:37" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A40" s="2">
         <v>44760.408561296295</v>
       </c>
@@ -7938,7 +7934,7 @@
       <c r="AJ40" s="3"/>
       <c r="AK40" s="3"/>
     </row>
-    <row r="41" spans="1:37" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A41" s="4">
         <v>44760.506068842587</v>
       </c>
@@ -8039,7 +8035,7 @@
       <c r="AJ41" s="5"/>
       <c r="AK41" s="5"/>
     </row>
-    <row r="42" spans="1:37" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A42" s="4">
         <v>44760.560046250001</v>
       </c>
@@ -8140,7 +8136,7 @@
       <c r="AJ42" s="5"/>
       <c r="AK42" s="5"/>
     </row>
-    <row r="43" spans="1:37" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A43" s="4">
         <v>44760.652184699073</v>
       </c>
@@ -8241,7 +8237,7 @@
       <c r="AJ43" s="5"/>
       <c r="AK43" s="5"/>
     </row>
-    <row r="44" spans="1:37" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A44" s="4">
         <v>44760.738571678245</v>
       </c>
@@ -8340,7 +8336,7 @@
       <c r="AJ44" s="5"/>
       <c r="AK44" s="5"/>
     </row>
-    <row r="45" spans="1:37" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A45" s="4">
         <v>44760.80759113426</v>
       </c>
@@ -8433,7 +8429,7 @@
       <c r="AJ45" s="5"/>
       <c r="AK45" s="5"/>
     </row>
-    <row r="46" spans="1:37" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A46" s="4">
         <v>44761.730599513889</v>
       </c>
@@ -8534,7 +8530,7 @@
       <c r="AJ46" s="5"/>
       <c r="AK46" s="5"/>
     </row>
-    <row r="47" spans="1:37" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A47" s="4">
         <v>44762.615112916668</v>
       </c>
@@ -8621,7 +8617,7 @@
       <c r="AJ47" s="5"/>
       <c r="AK47" s="5"/>
     </row>
-    <row r="48" spans="1:37" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A48" s="4">
         <v>44763.178732187502</v>
       </c>
@@ -8720,7 +8716,7 @@
       <c r="AJ48" s="5"/>
       <c r="AK48" s="5"/>
     </row>
-    <row r="49" spans="1:37" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A49" s="4">
         <v>44763.281734722223</v>
       </c>
@@ -8809,7 +8805,7 @@
       <c r="AJ49" s="5"/>
       <c r="AK49" s="5"/>
     </row>
-    <row r="50" spans="1:37" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A50" s="4">
         <v>44763.328978657402</v>
       </c>
@@ -8900,7 +8896,7 @@
       <c r="AJ50" s="5"/>
       <c r="AK50" s="5"/>
     </row>
-    <row r="51" spans="1:37" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A51" s="4">
         <v>44763.354922604165</v>
       </c>
@@ -8991,7 +8987,7 @@
       <c r="AJ51" s="5"/>
       <c r="AK51" s="5"/>
     </row>
-    <row r="52" spans="1:37" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A52" s="4">
         <v>44763.411183414355</v>
       </c>
@@ -9088,7 +9084,7 @@
       <c r="AJ52" s="5"/>
       <c r="AK52" s="5"/>
     </row>
-    <row r="53" spans="1:37" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A53" s="4">
         <v>44763.429527500004</v>
       </c>
@@ -9179,7 +9175,7 @@
       <c r="AJ53" s="5"/>
       <c r="AK53" s="5"/>
     </row>
-    <row r="54" spans="1:37" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A54" s="4">
         <v>44763.436787152779</v>
       </c>
@@ -9280,7 +9276,7 @@
       <c r="AJ54" s="5"/>
       <c r="AK54" s="5"/>
     </row>
-    <row r="55" spans="1:37" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A55" s="4">
         <v>44763.598419664355</v>
       </c>
@@ -9373,7 +9369,7 @@
       <c r="AJ55" s="5"/>
       <c r="AK55" s="5"/>
     </row>
-    <row r="56" spans="1:37" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A56" s="6">
         <v>44763.629912800927</v>
       </c>
@@ -9442,7 +9438,7 @@
       <c r="AJ56" s="7"/>
       <c r="AK56" s="7"/>
     </row>
-    <row r="57" spans="1:37" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A57" s="4">
         <v>44763.630420034722</v>
       </c>
@@ -9509,7 +9505,7 @@
       <c r="AJ57" s="5"/>
       <c r="AK57" s="5"/>
     </row>
-    <row r="58" spans="1:37" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A58" s="4">
         <v>44763.637512650464</v>
       </c>
@@ -9602,7 +9598,7 @@
       <c r="AJ58" s="5"/>
       <c r="AK58" s="5"/>
     </row>
-    <row r="59" spans="1:37" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A59" s="4">
         <v>44763.6417515625</v>
       </c>
@@ -9703,7 +9699,7 @@
       <c r="AJ59" s="5"/>
       <c r="AK59" s="5"/>
     </row>
-    <row r="60" spans="1:37" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A60" s="4">
         <v>44763.671027303237</v>
       </c>
@@ -9800,7 +9796,7 @@
       <c r="AJ60" s="5"/>
       <c r="AK60" s="5"/>
     </row>
-    <row r="61" spans="1:37" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A61" s="2">
         <v>44763.681260590281</v>
       </c>
@@ -9897,7 +9893,7 @@
       <c r="AJ61" s="3"/>
       <c r="AK61" s="3"/>
     </row>
-    <row r="62" spans="1:37" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A62" s="2">
         <v>44763.683786527778</v>
       </c>
@@ -9984,7 +9980,7 @@
       <c r="AJ62" s="3"/>
       <c r="AK62" s="3"/>
     </row>
-    <row r="63" spans="1:37" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A63" s="2">
         <v>44763.710078159726</v>
       </c>
@@ -10085,7 +10081,7 @@
       <c r="AJ63" s="3"/>
       <c r="AK63" s="3"/>
     </row>
-    <row r="64" spans="1:37" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A64" s="4">
         <v>44763.751637106485</v>
       </c>
@@ -10182,7 +10178,7 @@
       <c r="AJ64" s="5"/>
       <c r="AK64" s="5"/>
     </row>
-    <row r="65" spans="1:37" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A65" s="4">
         <v>44763.821287812505</v>
       </c>
@@ -10271,7 +10267,7 @@
       <c r="AJ65" s="5"/>
       <c r="AK65" s="5"/>
     </row>
-    <row r="66" spans="1:37" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A66" s="4">
         <v>44763.837111412038</v>
       </c>
@@ -10372,7 +10368,7 @@
       <c r="AJ66" s="5"/>
       <c r="AK66" s="5"/>
     </row>
-    <row r="67" spans="1:37" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A67" s="4">
         <v>44764.037820069439</v>
       </c>
@@ -10473,7 +10469,7 @@
       <c r="AJ67" s="5"/>
       <c r="AK67" s="5"/>
     </row>
-    <row r="68" spans="1:37" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A68" s="4">
         <v>44764.375806331023</v>
       </c>
@@ -10568,7 +10564,7 @@
       <c r="AJ68" s="5"/>
       <c r="AK68" s="5"/>
     </row>
-    <row r="69" spans="1:37" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A69" s="4">
         <v>44765.376572546294</v>
       </c>
@@ -10665,7 +10661,7 @@
       <c r="AJ69" s="5"/>
       <c r="AK69" s="5"/>
     </row>
-    <row r="70" spans="1:37" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A70" s="2">
         <v>44767.342136134263</v>
       </c>
@@ -10764,7 +10760,7 @@
       <c r="AJ70" s="3"/>
       <c r="AK70" s="3"/>
     </row>
-    <row r="71" spans="1:37" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A71" s="2">
         <v>44767.408527858795</v>
       </c>
@@ -10855,7 +10851,7 @@
       <c r="AJ71" s="3"/>
       <c r="AK71" s="3"/>
     </row>
-    <row r="72" spans="1:37" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A72" s="4">
         <v>44767.786165798607</v>
       </c>
@@ -10952,7 +10948,7 @@
       <c r="AJ72" s="5"/>
       <c r="AK72" s="5"/>
     </row>
-    <row r="73" spans="1:37" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A73" s="4">
         <v>44767.982161064814</v>
       </c>
@@ -11053,7 +11049,7 @@
       <c r="AJ73" s="5"/>
       <c r="AK73" s="5"/>
     </row>
-    <row r="74" spans="1:37" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A74" s="2">
         <v>44768.49386505787</v>
       </c>
@@ -11148,7 +11144,7 @@
       <c r="AJ74" s="3"/>
       <c r="AK74" s="3"/>
     </row>
-    <row r="75" spans="1:37" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A75" s="2">
         <v>44769.591317662038</v>
       </c>
@@ -11239,7 +11235,7 @@
       <c r="AJ75" s="3"/>
       <c r="AK75" s="3"/>
     </row>
-    <row r="76" spans="1:37" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A76" s="4">
         <v>44769.614276805558</v>
       </c>
@@ -11334,7 +11330,7 @@
       <c r="AJ76" s="5"/>
       <c r="AK76" s="5"/>
     </row>
-    <row r="77" spans="1:37" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A77" s="4">
         <v>44769.618707048612</v>
       </c>
@@ -11427,7 +11423,7 @@
       <c r="AJ77" s="5"/>
       <c r="AK77" s="5"/>
     </row>
-    <row r="78" spans="1:37" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A78" s="2">
         <v>44773.372072673606</v>
       </c>
@@ -11526,7 +11522,7 @@
       <c r="AJ78" s="3"/>
       <c r="AK78" s="3"/>
     </row>
-    <row r="79" spans="1:37" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A79" s="4">
         <v>44774.051016979167</v>
       </c>
@@ -11627,7 +11623,7 @@
       <c r="AJ79" s="5"/>
       <c r="AK79" s="5"/>
     </row>
-    <row r="80" spans="1:37" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A80" s="4">
         <v>44774.702917187504</v>
       </c>
@@ -11726,7 +11722,7 @@
       <c r="AJ80" s="5"/>
       <c r="AK80" s="5"/>
     </row>
-    <row r="81" spans="1:37" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A81" s="2">
         <v>44774.732120659726</v>
       </c>
@@ -11821,7 +11817,7 @@
       <c r="AJ81" s="3"/>
       <c r="AK81" s="3"/>
     </row>
-    <row r="82" spans="1:37" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A82" s="2">
         <v>44774.834338275468</v>
       </c>
@@ -11910,7 +11906,7 @@
       <c r="AJ82" s="3"/>
       <c r="AK82" s="3"/>
     </row>
-    <row r="83" spans="1:37" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A83" s="2">
         <v>44774.980285393518</v>
       </c>
@@ -11999,7 +11995,7 @@
       <c r="AJ83" s="3"/>
       <c r="AK83" s="3"/>
     </row>
-    <row r="84" spans="1:37" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A84" s="4">
         <v>44775.595694606483</v>
       </c>
@@ -12100,7 +12096,7 @@
       <c r="AJ84" s="5"/>
       <c r="AK84" s="5"/>
     </row>
-    <row r="85" spans="1:37" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A85" s="4">
         <v>44783.63758840278</v>
       </c>
@@ -12201,7 +12197,7 @@
       <c r="AJ85" s="5"/>
       <c r="AK85" s="5"/>
     </row>
-    <row r="86" spans="1:37" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A86" s="4">
         <v>44783.702055138885</v>
       </c>
@@ -12302,7 +12298,7 @@
       <c r="AJ86" s="5"/>
       <c r="AK86" s="5"/>
     </row>
-    <row r="87" spans="1:37" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A87" s="4">
         <v>44784.535158125</v>
       </c>
@@ -12401,7 +12397,7 @@
       <c r="AJ87" s="5"/>
       <c r="AK87" s="5"/>
     </row>
-    <row r="88" spans="1:37" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A88" s="4">
         <v>44784.55242501157</v>
       </c>
@@ -12502,7 +12498,7 @@
       <c r="AJ88" s="5"/>
       <c r="AK88" s="5"/>
     </row>
-    <row r="89" spans="1:37" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A89" s="4">
         <v>44785.054983888884</v>
       </c>
@@ -12597,7 +12593,7 @@
       <c r="AJ89" s="5"/>
       <c r="AK89" s="5"/>
     </row>
-    <row r="90" spans="1:37" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A90" s="2">
         <v>44795.453067465278</v>
       </c>
@@ -12690,7 +12686,7 @@
       <c r="AJ90" s="3"/>
       <c r="AK90" s="3"/>
     </row>
-    <row r="91" spans="1:37" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A91" s="4">
         <v>44797.964524814815</v>
       </c>
@@ -12789,7 +12785,7 @@
       <c r="AJ91" s="5"/>
       <c r="AK91" s="5"/>
     </row>
-    <row r="92" spans="1:37" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A92" s="4">
         <v>44799.579709247686</v>
       </c>
@@ -12887,37 +12883,37 @@
       <c r="AK92" s="5"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AK1" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
+  <autoFilter ref="A1:AK1"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:AE118"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="V1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="R1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Z6" sqref="Z6"/>
+      <selection pane="bottomLeft" activeCell="T6" sqref="T6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5546875" defaultRowHeight="15.75" customHeight="1" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" outlineLevelRow="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="12" width="18.88671875" customWidth="1"/>
-    <col min="13" max="13" width="39.33203125" hidden="1" customWidth="1"/>
-    <col min="14" max="14" width="16.33203125" customWidth="1"/>
-    <col min="15" max="15" width="88.109375" hidden="1" customWidth="1"/>
-    <col min="16" max="23" width="18.88671875" customWidth="1"/>
+    <col min="1" max="12" width="18.85546875" customWidth="1"/>
+    <col min="13" max="13" width="39.28515625" hidden="1" customWidth="1"/>
+    <col min="14" max="14" width="16.28515625" customWidth="1"/>
+    <col min="15" max="15" width="88.140625" hidden="1" customWidth="1"/>
+    <col min="16" max="23" width="18.85546875" customWidth="1"/>
     <col min="24" max="24" width="17" customWidth="1"/>
-    <col min="25" max="25" width="63.88671875" customWidth="1"/>
-    <col min="26" max="26" width="49.5546875" customWidth="1"/>
-    <col min="27" max="37" width="18.88671875" customWidth="1"/>
+    <col min="25" max="25" width="63.85546875" customWidth="1"/>
+    <col min="26" max="26" width="49.5703125" customWidth="1"/>
+    <col min="27" max="37" width="18.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" ht="13.2" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:31" ht="12.75" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -13012,7 +13008,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:31" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A2" s="8">
         <v>44756.743593946754</v>
       </c>
@@ -13104,7 +13100,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="3" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:31" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A3" s="8">
         <v>44756.746476273147</v>
       </c>
@@ -13196,7 +13192,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="4" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:31" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A4" s="8">
         <v>44756.751307071754</v>
       </c>
@@ -13276,7 +13272,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="5" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:31" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A5" s="8">
         <v>44756.751650844904</v>
       </c>
@@ -13368,7 +13364,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="6" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:31" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A6" s="8">
         <v>44756.756480439813</v>
       </c>
@@ -13457,7 +13453,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="7" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:31" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A7" s="8">
         <v>44756.765615289347</v>
       </c>
@@ -13552,7 +13548,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="8" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:31" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A8" s="8">
         <v>44756.77190482639</v>
       </c>
@@ -13647,7 +13643,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="9" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:31" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A9" s="8">
         <v>44756.781270081017</v>
       </c>
@@ -13739,7 +13735,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="10" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:31" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A10" s="8">
         <v>44756.784393831018</v>
       </c>
@@ -13819,7 +13815,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="11" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:31" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A11" s="8">
         <v>44756.788800416667</v>
       </c>
@@ -13899,7 +13895,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="12" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:31" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A12" s="8">
         <v>44756.791462858797</v>
       </c>
@@ -13982,7 +13978,7 @@
         <v>954</v>
       </c>
     </row>
-    <row r="13" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:31" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A13" s="8">
         <v>44756.795764756942</v>
       </c>
@@ -14071,7 +14067,7 @@
         <v>964</v>
       </c>
     </row>
-    <row r="14" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:31" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A14" s="8">
         <v>44756.798618148146</v>
       </c>
@@ -14163,7 +14159,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="15" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:31" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A15" s="8">
         <v>44756.799106678242</v>
       </c>
@@ -14246,7 +14242,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="16" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:31" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A16" s="8">
         <v>44756.81055918982</v>
       </c>
@@ -14341,7 +14337,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="17" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:31" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A17" s="8">
         <v>44756.816295104167</v>
       </c>
@@ -14433,7 +14429,7 @@
         <v>975</v>
       </c>
     </row>
-    <row r="18" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:31" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A18" s="8">
         <v>44756.827279050922</v>
       </c>
@@ -14513,7 +14509,7 @@
         <v>982</v>
       </c>
     </row>
-    <row r="19" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:31" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A19" s="8">
         <v>44756.836429988427</v>
       </c>
@@ -14596,7 +14592,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="20" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:31" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A20" s="8">
         <v>44756.844614560185</v>
       </c>
@@ -14679,7 +14675,7 @@
         <v>989</v>
       </c>
     </row>
-    <row r="21" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:31" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A21" s="8">
         <v>44756.871095520837</v>
       </c>
@@ -14765,7 +14761,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="22" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:31" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A22" s="8">
         <v>44756.915538368055</v>
       </c>
@@ -14857,7 +14853,7 @@
         <v>999</v>
       </c>
     </row>
-    <row r="23" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:31" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A23" s="8">
         <v>44756.915725775463</v>
       </c>
@@ -14952,7 +14948,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="24" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:31" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A24" s="8">
         <v>44756.921014201391</v>
       </c>
@@ -15041,7 +15037,7 @@
         <v>1007</v>
       </c>
     </row>
-    <row r="25" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:31" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A25" s="8">
         <v>44756.941017210644</v>
       </c>
@@ -15136,7 +15132,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="26" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:31" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A26" s="8">
         <v>44756.942555740738</v>
       </c>
@@ -15228,7 +15224,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="27" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:31" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A27" s="8">
         <v>44756.949555925923</v>
       </c>
@@ -15323,7 +15319,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="28" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:31" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A28" s="8">
         <v>44756.97487351852</v>
       </c>
@@ -15415,7 +15411,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="29" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:31" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A29" s="8">
         <v>44756.99139891204</v>
       </c>
@@ -15507,7 +15503,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="30" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:31" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A30" s="8">
         <v>44756.996441898147</v>
       </c>
@@ -15602,7 +15598,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="31" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:31" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A31" s="8">
         <v>44756.998882719912</v>
       </c>
@@ -15688,7 +15684,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="32" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:31" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A32" s="8">
         <v>44757.336282847224</v>
       </c>
@@ -15774,7 +15770,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="33" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:31" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A33" s="8">
         <v>44757.353061064816</v>
       </c>
@@ -15866,7 +15862,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="34" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:31" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A34" s="8">
         <v>44757.367554224533</v>
       </c>
@@ -15949,7 +15945,7 @@
         <v>1024</v>
       </c>
     </row>
-    <row r="35" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:31" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A35" s="8">
         <v>44757.37340394676</v>
       </c>
@@ -16038,7 +16034,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="36" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:31" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A36" s="8">
         <v>44757.424635173607</v>
       </c>
@@ -16118,7 +16114,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="37" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:31" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A37" s="8">
         <v>44757.425247453706</v>
       </c>
@@ -16213,7 +16209,7 @@
         <v>1034</v>
       </c>
     </row>
-    <row r="38" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:31" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A38" s="8">
         <v>44757.485260335648</v>
       </c>
@@ -16266,7 +16262,7 @@
         <v>291</v>
       </c>
       <c r="T38" s="1" t="s">
-        <v>1225</v>
+        <v>1224</v>
       </c>
       <c r="U38" s="1" t="s">
         <v>74</v>
@@ -16302,7 +16298,7 @@
         <v>1044</v>
       </c>
     </row>
-    <row r="39" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:31" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A39" s="8">
         <v>44757.514283750003</v>
       </c>
@@ -16385,7 +16381,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="40" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:31" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A40" s="8">
         <v>44757.520848252316</v>
       </c>
@@ -16465,7 +16461,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="41" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:31" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A41" s="8">
         <v>44757.537129490738</v>
       </c>
@@ -16557,7 +16553,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="42" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:31" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A42" s="8">
         <v>44757.570692685185</v>
       </c>
@@ -16652,7 +16648,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="43" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:31" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A43" s="8">
         <v>44757.577583460647</v>
       </c>
@@ -16744,7 +16740,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="44" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:31" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A44" s="8">
         <v>44757.656166469911</v>
       </c>
@@ -16827,7 +16823,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="45" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:31" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A45" s="8">
         <v>44757.775384513894</v>
       </c>
@@ -16907,7 +16903,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="46" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:31" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A46" s="8">
         <v>44757.795752696758</v>
       </c>
@@ -17002,7 +16998,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="47" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:31" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A47" s="8">
         <v>44757.842575543982</v>
       </c>
@@ -17058,7 +17054,7 @@
         <v>48</v>
       </c>
       <c r="T47" s="1" t="s">
-        <v>1224</v>
+        <v>1215</v>
       </c>
       <c r="U47" s="1" t="s">
         <v>41</v>
@@ -17091,7 +17087,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="48" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:31" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A48" s="8">
         <v>44758.725458171291</v>
       </c>
@@ -17174,7 +17170,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="49" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:31" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A49" s="8">
         <v>44759.705415173608</v>
       </c>
@@ -17260,7 +17256,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="50" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:31" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A50" s="8">
         <v>44760.010943865738</v>
       </c>
@@ -17352,7 +17348,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="51" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:31" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A51" s="8">
         <v>44760.399100844908</v>
       </c>
@@ -17438,7 +17434,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="52" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:31" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A52" s="8">
         <v>44760.408561296295</v>
       </c>
@@ -17530,7 +17526,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="53" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:31" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A53" s="8">
         <v>44760.506068842587</v>
       </c>
@@ -17625,7 +17621,7 @@
         <v>503</v>
       </c>
     </row>
-    <row r="54" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:31" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A54" s="8">
         <v>44760.55148765046</v>
       </c>
@@ -17714,7 +17710,7 @@
         <v>1062</v>
       </c>
     </row>
-    <row r="55" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:31" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A55" s="8">
         <v>44760.560046250001</v>
       </c>
@@ -17809,7 +17805,7 @@
         <v>516</v>
       </c>
     </row>
-    <row r="56" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:31" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A56" s="8">
         <v>44760.628381087961</v>
       </c>
@@ -17904,7 +17900,7 @@
         <v>1073</v>
       </c>
     </row>
-    <row r="57" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:31" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A57" s="8">
         <v>44760.652184699073</v>
       </c>
@@ -17999,7 +17995,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="58" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:31" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A58" s="8">
         <v>44760.65833395833</v>
       </c>
@@ -18082,7 +18078,7 @@
         <v>1081</v>
       </c>
     </row>
-    <row r="59" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:31" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A59" s="8">
         <v>44760.738571678245</v>
       </c>
@@ -18174,7 +18170,7 @@
         <v>539</v>
       </c>
     </row>
-    <row r="60" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:31" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A60" s="8">
         <v>44760.80759113426</v>
       </c>
@@ -18257,7 +18253,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="61" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:31" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A61" s="8">
         <v>44761.400200868055</v>
       </c>
@@ -18352,7 +18348,7 @@
         <v>1091</v>
       </c>
     </row>
-    <row r="62" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:31" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A62" s="8">
         <v>44761.730599513889</v>
       </c>
@@ -18447,7 +18443,7 @@
         <v>559</v>
       </c>
     </row>
-    <row r="63" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:31" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A63" s="8">
         <v>44762.615112916668</v>
       </c>
@@ -18521,7 +18517,7 @@
         <v>563</v>
       </c>
     </row>
-    <row r="64" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:31" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A64" s="8">
         <v>44762.778823912042</v>
       </c>
@@ -18613,7 +18609,7 @@
         <v>1102</v>
       </c>
     </row>
-    <row r="65" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:31" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A65" s="8">
         <v>44763.178732187502</v>
       </c>
@@ -18705,7 +18701,7 @@
         <v>574</v>
       </c>
     </row>
-    <row r="66" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:31" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A66" s="8">
         <v>44763.281734722223</v>
       </c>
@@ -18782,7 +18778,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="67" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:31" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A67" s="8">
         <v>44763.328978657402</v>
       </c>
@@ -18862,7 +18858,7 @@
         <v>588</v>
       </c>
     </row>
-    <row r="68" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:31" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A68" s="8">
         <v>44763.354922604165</v>
       </c>
@@ -18942,7 +18938,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="69" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:31" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A69" s="8">
         <v>44763.411183414355</v>
       </c>
@@ -19031,7 +19027,7 @@
         <v>605</v>
       </c>
     </row>
-    <row r="70" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:31" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A70" s="8">
         <v>44763.429527500004</v>
       </c>
@@ -19111,7 +19107,7 @@
         <v>611</v>
       </c>
     </row>
-    <row r="71" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:31" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A71" s="8">
         <v>44763.436787152779</v>
       </c>
@@ -19206,7 +19202,7 @@
         <v>622</v>
       </c>
     </row>
-    <row r="72" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:31" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A72" s="8">
         <v>44763.598419664355</v>
       </c>
@@ -19289,7 +19285,7 @@
         <v>629</v>
       </c>
     </row>
-    <row r="73" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:31" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A73" s="8">
         <v>44763.637512650464</v>
       </c>
@@ -19372,7 +19368,7 @@
         <v>644</v>
       </c>
     </row>
-    <row r="74" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:31" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A74" s="8">
         <v>44763.6417515625</v>
       </c>
@@ -19467,7 +19463,7 @@
         <v>657</v>
       </c>
     </row>
-    <row r="75" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:31" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A75" s="8">
         <v>44763.663818275461</v>
       </c>
@@ -19547,7 +19543,7 @@
         <v>1109</v>
       </c>
     </row>
-    <row r="76" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:31" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A76" s="8">
         <v>44763.671027303237</v>
       </c>
@@ -19636,7 +19632,7 @@
         <v>667</v>
       </c>
     </row>
-    <row r="77" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:31" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A77" s="8">
         <v>44763.681260590281</v>
       </c>
@@ -19725,7 +19721,7 @@
         <v>675</v>
       </c>
     </row>
-    <row r="78" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:31" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A78" s="8">
         <v>44763.683786527778</v>
       </c>
@@ -19799,7 +19795,7 @@
         <v>680</v>
       </c>
     </row>
-    <row r="79" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:31" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A79" s="8">
         <v>44763.710078159726</v>
       </c>
@@ -19894,7 +19890,7 @@
         <v>693</v>
       </c>
     </row>
-    <row r="80" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:31" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A80" s="8">
         <v>44763.751637106485</v>
       </c>
@@ -19983,7 +19979,7 @@
         <v>705</v>
       </c>
     </row>
-    <row r="81" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:31" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A81" s="8">
         <v>44763.75527415509</v>
       </c>
@@ -20075,7 +20071,7 @@
         <v>1119</v>
       </c>
     </row>
-    <row r="82" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:31" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A82" s="8">
         <v>44763.821287812505</v>
       </c>
@@ -20152,7 +20148,7 @@
         <v>711</v>
       </c>
     </row>
-    <row r="83" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:31" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A83" s="8">
         <v>44763.837111412038</v>
       </c>
@@ -20247,7 +20243,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="84" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:31" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A84" s="8">
         <v>44764.037820069439</v>
       </c>
@@ -20342,7 +20338,7 @@
         <v>728</v>
       </c>
     </row>
-    <row r="85" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:31" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A85" s="8">
         <v>44764.375806331023</v>
       </c>
@@ -20428,7 +20424,7 @@
         <v>736</v>
       </c>
     </row>
-    <row r="86" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:31" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A86" s="8">
         <v>44764.440489525463</v>
       </c>
@@ -20514,7 +20510,7 @@
         <v>1126</v>
       </c>
     </row>
-    <row r="87" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:31" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A87" s="8">
         <v>44765.376572546294</v>
       </c>
@@ -20603,7 +20599,7 @@
         <v>741</v>
       </c>
     </row>
-    <row r="88" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:31" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A88" s="8">
         <v>44767.342136134263</v>
       </c>
@@ -20695,7 +20691,7 @@
         <v>749</v>
       </c>
     </row>
-    <row r="89" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:31" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A89" s="8">
         <v>44767.408527858795</v>
       </c>
@@ -20775,7 +20771,7 @@
         <v>758</v>
       </c>
     </row>
-    <row r="90" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:31" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A90" s="8">
         <v>44767.786165798607</v>
       </c>
@@ -20864,7 +20860,7 @@
         <v>768</v>
       </c>
     </row>
-    <row r="91" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:31" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A91" s="8">
         <v>44767.982161064814</v>
       </c>
@@ -20959,7 +20955,7 @@
         <v>778</v>
       </c>
     </row>
-    <row r="92" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:31" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A92" s="8">
         <v>44768.49386505787</v>
       </c>
@@ -21045,7 +21041,7 @@
         <v>785</v>
       </c>
     </row>
-    <row r="93" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:31" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A93" s="8">
         <v>44768.961886979167</v>
       </c>
@@ -21125,7 +21121,7 @@
         <v>1134</v>
       </c>
     </row>
-    <row r="94" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:31" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A94" s="8">
         <v>44769.551213599538</v>
       </c>
@@ -21205,7 +21201,7 @@
         <v>1139</v>
       </c>
     </row>
-    <row r="95" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:31" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A95" s="8">
         <v>44769.591317662038</v>
       </c>
@@ -21285,7 +21281,7 @@
         <v>792</v>
       </c>
     </row>
-    <row r="96" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:31" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A96" s="8">
         <v>44769.614276805558</v>
       </c>
@@ -21371,7 +21367,7 @@
         <v>799</v>
       </c>
     </row>
-    <row r="97" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:31" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A97" s="8">
         <v>44769.618707048612</v>
       </c>
@@ -21454,7 +21450,7 @@
         <v>807</v>
       </c>
     </row>
-    <row r="98" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:31" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A98" s="8">
         <v>44772.587381527774</v>
       </c>
@@ -21543,7 +21539,7 @@
         <v>1150</v>
       </c>
     </row>
-    <row r="99" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:31" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A99" s="8">
         <v>44773.372072673606</v>
       </c>
@@ -21635,7 +21631,7 @@
         <v>816</v>
       </c>
     </row>
-    <row r="100" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:31" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A100" s="8">
         <v>44774.051016979167</v>
       </c>
@@ -21730,7 +21726,7 @@
         <v>827</v>
       </c>
     </row>
-    <row r="101" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:31" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A101" s="8">
         <v>44774.702917187504</v>
       </c>
@@ -21822,7 +21818,7 @@
         <v>836</v>
       </c>
     </row>
-    <row r="102" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:31" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A102" s="8">
         <v>44774.732120659726</v>
       </c>
@@ -21908,7 +21904,7 @@
         <v>844</v>
       </c>
     </row>
-    <row r="103" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:31" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A103" s="8">
         <v>44774.834338275468</v>
       </c>
@@ -21985,7 +21981,7 @@
         <v>852</v>
       </c>
     </row>
-    <row r="104" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:31" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A104" s="8">
         <v>44774.980285393518</v>
       </c>
@@ -22062,7 +22058,7 @@
         <v>858</v>
       </c>
     </row>
-    <row r="105" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:31" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A105" s="8">
         <v>44775.595694606483</v>
       </c>
@@ -22157,7 +22153,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="106" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:31" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A106" s="8">
         <v>44783.63758840278</v>
       </c>
@@ -22252,7 +22248,7 @@
         <v>879</v>
       </c>
     </row>
-    <row r="107" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:31" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A107" s="8">
         <v>44783.682308530093</v>
       </c>
@@ -22344,7 +22340,7 @@
         <v>1158</v>
       </c>
     </row>
-    <row r="108" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:31" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A108" s="8">
         <v>44783.702055138885</v>
       </c>
@@ -22403,7 +22399,7 @@
         <v>888</v>
       </c>
       <c r="T108" s="1" t="s">
-        <v>1226</v>
+        <v>1225</v>
       </c>
       <c r="U108" s="1" t="s">
         <v>41</v>
@@ -22439,7 +22435,7 @@
         <v>894</v>
       </c>
     </row>
-    <row r="109" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:31" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A109" s="8">
         <v>44784.349818946765</v>
       </c>
@@ -22531,7 +22527,7 @@
         <v>1169</v>
       </c>
     </row>
-    <row r="110" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:31" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A110" s="8">
         <v>44784.535158125</v>
       </c>
@@ -22590,7 +22586,7 @@
         <v>291</v>
       </c>
       <c r="T110" s="1" t="s">
-        <v>1227</v>
+        <v>1226</v>
       </c>
       <c r="U110" s="1" t="s">
         <v>41</v>
@@ -22623,7 +22619,7 @@
         <v>902</v>
       </c>
     </row>
-    <row r="111" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:31" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A111" s="8">
         <v>44784.55242501157</v>
       </c>
@@ -22718,7 +22714,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="112" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:31" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A112" s="8">
         <v>44785.054983888884</v>
       </c>
@@ -22804,7 +22800,7 @@
         <v>919</v>
       </c>
     </row>
-    <row r="113" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:31" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A113" s="8">
         <v>44785.523622499997</v>
       </c>
@@ -22884,7 +22880,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="114" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:31" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A114" s="8">
         <v>44789.386663738427</v>
       </c>
@@ -22976,7 +22972,7 @@
         <v>1183</v>
       </c>
     </row>
-    <row r="115" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:31" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A115" s="8">
         <v>44795.453067465278</v>
       </c>
@@ -23059,7 +23055,7 @@
         <v>926</v>
       </c>
     </row>
-    <row r="116" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:31" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A116" s="8">
         <v>44797.964524814815</v>
       </c>
@@ -23151,7 +23147,7 @@
         <v>936</v>
       </c>
     </row>
-    <row r="117" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:31" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A117" s="8">
         <v>44798.701526782403</v>
       </c>
@@ -23240,7 +23236,7 @@
         <v>1191</v>
       </c>
     </row>
-    <row r="118" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:31" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A118" s="8">
         <v>44799.579709247686</v>
       </c>
@@ -23330,13 +23326,13 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AK118" xr:uid="{00000000-0009-0000-0000-000002000000}"/>
+  <autoFilter ref="A1:AK118"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
     <outlinePr summaryRight="0"/>
@@ -23348,21 +23344,21 @@
       <selection pane="bottomLeft" activeCell="P32" sqref="P32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5546875" defaultRowHeight="15.75" customHeight="1" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" outlineLevelRow="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="11" width="18.88671875" customWidth="1"/>
-    <col min="12" max="12" width="42.109375" customWidth="1"/>
-    <col min="13" max="13" width="26.33203125" customWidth="1"/>
-    <col min="14" max="14" width="99.44140625" customWidth="1"/>
-    <col min="15" max="15" width="48.33203125" customWidth="1"/>
-    <col min="16" max="16" width="16.88671875" customWidth="1"/>
-    <col min="17" max="17" width="135.6640625" customWidth="1"/>
-    <col min="18" max="18" width="6.44140625" customWidth="1"/>
-    <col min="19" max="19" width="107.33203125" customWidth="1"/>
-    <col min="20" max="37" width="18.88671875" customWidth="1"/>
+    <col min="1" max="11" width="18.85546875" customWidth="1"/>
+    <col min="12" max="12" width="42.140625" customWidth="1"/>
+    <col min="13" max="13" width="26.28515625" customWidth="1"/>
+    <col min="14" max="14" width="99.42578125" customWidth="1"/>
+    <col min="15" max="15" width="48.28515625" customWidth="1"/>
+    <col min="16" max="16" width="16.85546875" customWidth="1"/>
+    <col min="17" max="17" width="135.7109375" customWidth="1"/>
+    <col min="18" max="18" width="6.42578125" customWidth="1"/>
+    <col min="19" max="19" width="107.28515625" customWidth="1"/>
+    <col min="20" max="37" width="18.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" ht="13.2" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:31" ht="12.75" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -23457,7 +23453,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:31" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A2" s="8">
         <v>44756.791462858797</v>
       </c>
@@ -23540,7 +23536,7 @@
         <v>954</v>
       </c>
     </row>
-    <row r="3" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:31" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A3" s="8">
         <v>44756.795764756942</v>
       </c>
@@ -23629,7 +23625,7 @@
         <v>964</v>
       </c>
     </row>
-    <row r="4" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:31" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A4" s="8">
         <v>44756.816295104167</v>
       </c>
@@ -23721,7 +23717,7 @@
         <v>975</v>
       </c>
     </row>
-    <row r="5" spans="1:31" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:31" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="8">
         <v>44756.827279050922</v>
       </c>
@@ -23801,7 +23797,7 @@
         <v>982</v>
       </c>
     </row>
-    <row r="6" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:31" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A6" s="8">
         <v>44756.844614560185</v>
       </c>
@@ -23884,7 +23880,7 @@
         <v>989</v>
       </c>
     </row>
-    <row r="7" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:31" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A7" s="8">
         <v>44756.915538368055</v>
       </c>
@@ -23976,7 +23972,7 @@
         <v>999</v>
       </c>
     </row>
-    <row r="8" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:31" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A8" s="8">
         <v>44756.921014201391</v>
       </c>
@@ -24065,7 +24061,7 @@
         <v>1007</v>
       </c>
     </row>
-    <row r="9" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:31" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A9" s="8">
         <v>44756.97487351852</v>
       </c>
@@ -24157,7 +24153,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="10" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:31" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A10" s="8">
         <v>44757.367554224533</v>
       </c>
@@ -24240,7 +24236,7 @@
         <v>1024</v>
       </c>
     </row>
-    <row r="11" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:31" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A11" s="8">
         <v>44757.425247453706</v>
       </c>
@@ -24335,7 +24331,7 @@
         <v>1034</v>
       </c>
     </row>
-    <row r="12" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:31" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A12" s="8">
         <v>44757.485260335648</v>
       </c>
@@ -24424,7 +24420,7 @@
         <v>1044</v>
       </c>
     </row>
-    <row r="13" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:31" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A13" s="8">
         <v>44757.577583460647</v>
       </c>
@@ -24516,7 +24512,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="14" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:31" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A14" s="8">
         <v>44759.705415173608</v>
       </c>
@@ -24602,7 +24598,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="15" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:31" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A15" s="8">
         <v>44760.55148765046</v>
       </c>
@@ -24691,7 +24687,7 @@
         <v>1062</v>
       </c>
     </row>
-    <row r="16" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:31" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A16" s="8">
         <v>44760.628381087961</v>
       </c>
@@ -24786,7 +24782,7 @@
         <v>1073</v>
       </c>
     </row>
-    <row r="17" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:31" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A17" s="8">
         <v>44760.65833395833</v>
       </c>
@@ -24869,7 +24865,7 @@
         <v>1081</v>
       </c>
     </row>
-    <row r="18" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:31" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A18" s="8">
         <v>44761.400200868055</v>
       </c>
@@ -24964,7 +24960,7 @@
         <v>1091</v>
       </c>
     </row>
-    <row r="19" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:31" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A19" s="8">
         <v>44762.778823912042</v>
       </c>
@@ -25056,7 +25052,7 @@
         <v>1102</v>
       </c>
     </row>
-    <row r="20" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:31" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A20" s="8">
         <v>44763.663818275461</v>
       </c>
@@ -25136,7 +25132,7 @@
         <v>1109</v>
       </c>
     </row>
-    <row r="21" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:31" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A21" s="8">
         <v>44763.75527415509</v>
       </c>
@@ -25228,7 +25224,7 @@
         <v>1119</v>
       </c>
     </row>
-    <row r="22" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:31" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A22" s="8">
         <v>44764.440489525463</v>
       </c>
@@ -25314,7 +25310,7 @@
         <v>1126</v>
       </c>
     </row>
-    <row r="23" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:31" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A23" s="8">
         <v>44768.961886979167</v>
       </c>
@@ -25394,7 +25390,7 @@
         <v>1134</v>
       </c>
     </row>
-    <row r="24" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:31" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A24" s="8">
         <v>44769.551213599538</v>
       </c>
@@ -25474,7 +25470,7 @@
         <v>1139</v>
       </c>
     </row>
-    <row r="25" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:31" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A25" s="8">
         <v>44772.587381527774</v>
       </c>
@@ -25563,7 +25559,7 @@
         <v>1150</v>
       </c>
     </row>
-    <row r="26" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:31" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A26" s="8">
         <v>44783.682308530093</v>
       </c>
@@ -25655,7 +25651,7 @@
         <v>1158</v>
       </c>
     </row>
-    <row r="27" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:31" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A27" s="8">
         <v>44784.349818946765</v>
       </c>
@@ -25747,7 +25743,7 @@
         <v>1169</v>
       </c>
     </row>
-    <row r="28" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:31" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A28" s="8">
         <v>44785.523622499997</v>
       </c>
@@ -25827,7 +25823,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="29" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:31" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A29" s="8">
         <v>44789.386663738427</v>
       </c>
@@ -25919,7 +25915,7 @@
         <v>1183</v>
       </c>
     </row>
-    <row r="30" spans="1:31" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:31" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A30" s="8">
         <v>44798.701526782403</v>
       </c>
@@ -26009,7 +26005,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AE30" xr:uid="{00000000-0009-0000-0000-000003000000}"/>
+  <autoFilter ref="A1:AE30"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
</xml_diff>